<commit_message>
Documentatie TestLink Lab 3
</commit_message>
<xml_diff>
--- a/01_Tasks/01_Tasks/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
+++ b/01_Tasks/01_Tasks/Docs/Lab2/Lab02_BBT_TCs_Form.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5CD46F-8C98-4F13-99F3-B1C92809E136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -13,7 +12,7 @@
     <sheet name="F01.BVA" sheetId="3" r:id="rId3"/>
     <sheet name="BBT-TCs" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,12 +31,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="H22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="M22" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,9 +339,6 @@
     <t>vom alege valorile description si startDate</t>
   </si>
   <si>
-    <t>decription este un string cu lungimea intre 1 si 255 de caractere, iar startDate trebuie sa ia valori intre 1970-01-01 si 2024-12-31</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -433,13 +429,7 @@
     <t>date = 2020-01-01</t>
   </si>
   <si>
-    <t>start is in (1969-12-31, 2050-01-01)</t>
-  </si>
-  <si>
     <t>date = 2050-01-01</t>
-  </si>
-  <si>
-    <t>date = 1919-12-31</t>
   </si>
   <si>
     <t>date = 2049-12-31</t>
@@ -488,9 +478,6 @@
     <t>length = 0, title = ""</t>
   </si>
   <si>
-    <t>length = 1, title = "S"</t>
-  </si>
-  <si>
     <t>length = 256, title = "wLhIUEnLeKNcsrv7oFQqpr2gznG41jQdaWE5MYp1x2Z88PEuaCegF3dSr3ScuuwzzFfT5Fj6Zah8etTUXrRiUau9qfLJZxqwqMoaDv6TT6mG8V2V20BrOlYlV1w2A50sREW5YFRA5N4cY1UMF7NMZN5KTeSCWskqlz5gKbdFbQaMj6P2ZZ3xqHlBH4eDfbrpKD6RJB3i4rASxpJ3RSNNMX0rG4uYJrnuCWlkFiEtjzd3yhVrkIlIwIpw4U9oH6Yt"</t>
   </si>
   <si>
@@ -507,12 +494,24 @@
   </si>
   <si>
     <t>T</t>
+  </si>
+  <si>
+    <t>decription este un string cu lungimea intre 1 si 255 de caractere, iar startDate trebuie sa ia valori intre 2020-01-01 si 2050-12-31</t>
+  </si>
+  <si>
+    <t>start is in (2019-12-31, 2050-01-01)</t>
+  </si>
+  <si>
+    <t>date = 2019-12-31</t>
+  </si>
+  <si>
+    <t>length = 1, title = "T"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1283,216 +1282,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1504,6 +1293,216 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1541,7 +1540,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3C835C-6E80-4BEA-7429-29B22B5626FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BF3C835C-6E80-4BEA-7429-29B22B5626FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1602,7 +1601,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D6363F9-9292-B503-59E7-D499E2294132}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4D6363F9-9292-B503-59E7-D499E2294132}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1649,9 +1648,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1689,9 +1688,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1726,7 +1725,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1761,7 +1760,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1934,14 +1933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1955,12 +1954,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="62"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69"/>
       <c r="H1" s="32" t="s">
         <v>1</v>
       </c>
@@ -1968,11 +1967,11 @@
       <c r="J1" s="32"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H2" s="63" t="s">
+      <c r="H2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="H3" s="2"/>
@@ -2092,7 +2091,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O22" s="1"/>
     </row>
@@ -2112,7 +2111,7 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2126,14 +2125,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:N25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2154,40 +2153,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="67" t="s">
-        <v>104</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="69"/>
+      <c r="B3" s="80" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="82"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="83" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="G5" s="71" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="G5" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
@@ -2202,36 +2201,36 @@
       <c r="E6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="80" t="s">
+      <c r="H6" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="84" t="s">
+      <c r="I6" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="83" t="s">
+      <c r="J6" s="73"/>
+      <c r="K6" s="73"/>
+      <c r="L6" s="73"/>
+      <c r="M6" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="N6" s="83"/>
+      <c r="N6" s="71"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="65" t="s">
-        <v>105</v>
+      <c r="C7" s="78" t="s">
+        <v>102</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="73"/>
-      <c r="H7" s="81"/>
+        <v>103</v>
+      </c>
+      <c r="G7" s="86"/>
+      <c r="H7" s="92"/>
       <c r="I7" s="33"/>
       <c r="J7" s="36"/>
       <c r="K7" s="36"/>
@@ -2243,13 +2242,13 @@
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="88"/>
       <c r="D8" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="81"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="92"/>
       <c r="I8" s="33"/>
       <c r="J8" s="36"/>
       <c r="K8" s="36"/>
@@ -2261,40 +2260,40 @@
       <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="66"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="74"/>
-      <c r="H9" s="82"/>
+        <v>104</v>
+      </c>
+      <c r="G9" s="87"/>
+      <c r="H9" s="93"/>
       <c r="I9" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J9" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="L9" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="L9" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="M9" s="84" t="s">
+      <c r="M9" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="86"/>
+      <c r="N9" s="74"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="65" t="s">
-        <v>95</v>
+      <c r="C10" s="78" t="s">
+        <v>94</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="34"/>
@@ -2309,9 +2308,9 @@
       <c r="B11" s="4">
         <v>5</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" s="4"/>
       <c r="G11" s="14">
@@ -2321,30 +2320,30 @@
         <v>2</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K11" s="39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L11" s="2">
         <v>1</v>
       </c>
-      <c r="M11" s="76" t="s">
-        <v>89</v>
-      </c>
-      <c r="N11" s="77"/>
+      <c r="M11" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="N11" s="90"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>6</v>
       </c>
-      <c r="C12" s="66"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G12" s="10">
         <v>2</v>
@@ -2353,27 +2352,27 @@
         <v>3</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J12" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="K12" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L12" s="9">
         <v>1</v>
       </c>
-      <c r="M12" s="78" t="s">
-        <v>73</v>
-      </c>
-      <c r="N12" s="79"/>
+      <c r="M12" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="N12" s="76"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>7</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="78" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="4"/>
@@ -2385,7 +2384,7 @@
         <v>5</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J13" s="39">
         <v>47463</v>
@@ -2396,16 +2395,16 @@
       <c r="L13" s="2">
         <v>1</v>
       </c>
-      <c r="M13" s="76" t="s">
-        <v>90</v>
-      </c>
-      <c r="N13" s="77"/>
+      <c r="M13" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="90"/>
     </row>
     <row r="14" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <v>8</v>
       </c>
-      <c r="C14" s="66"/>
+      <c r="C14" s="79"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="G14" s="10">
@@ -2415,7 +2414,7 @@
         <v>6</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="J14" s="40">
         <v>45403</v>
@@ -2426,16 +2425,16 @@
       <c r="L14" s="9">
         <v>1</v>
       </c>
-      <c r="M14" s="78" t="s">
-        <v>74</v>
-      </c>
-      <c r="N14" s="79"/>
+      <c r="M14" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="N14" s="76"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
         <v>9</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="77" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="4"/>
@@ -2446,14 +2445,14 @@
       <c r="J15" s="9"/>
       <c r="K15" s="39"/>
       <c r="L15" s="2"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="79"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="76"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>10</v>
       </c>
-      <c r="C16" s="64"/>
+      <c r="C16" s="77"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="G16" s="10"/>
@@ -2462,14 +2461,14 @@
       <c r="J16" s="9"/>
       <c r="K16" s="39"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="79"/>
+      <c r="M16" s="75"/>
+      <c r="N16" s="76"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>11</v>
       </c>
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="77" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="4"/>
@@ -2479,7 +2478,7 @@
       <c r="B18" s="4">
         <v>12</v>
       </c>
-      <c r="C18" s="64"/>
+      <c r="C18" s="77"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
@@ -2487,7 +2486,7 @@
       <c r="B19" s="4">
         <v>13</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="77" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="4"/>
@@ -2497,7 +2496,7 @@
       <c r="B20" s="4">
         <v>14</v>
       </c>
-      <c r="C20" s="64"/>
+      <c r="C20" s="77"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
@@ -2514,11 +2513,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C13:C14"/>
@@ -2535,6 +2529,11 @@
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="H6:H9"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2542,14 +2541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:M15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2571,42 +2570,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B3" s="67" t="s">
-        <v>108</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="69"/>
+      <c r="B3" s="80" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="82"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="3"/>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
-      <c r="N5" s="71"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
     </row>
     <row r="6" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -2619,65 +2618,65 @@
         <v>30</v>
       </c>
       <c r="E6" s="6"/>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="85" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="72" t="s">
+      <c r="H6" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="72" t="s">
+      <c r="I6" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="80" t="s">
+      <c r="J6" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="94" t="s">
+      <c r="K6" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="L6" s="98"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="94" t="s">
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="95"/>
+      <c r="P6" s="102"/>
     </row>
     <row r="7" spans="2:16" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="65">
+      <c r="B7" s="78">
         <v>1</v>
       </c>
-      <c r="C7" s="87" t="s">
-        <v>109</v>
+      <c r="C7" s="103" t="s">
+        <v>106</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="82"/>
+        <v>107</v>
+      </c>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="93"/>
       <c r="K7" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L7" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="N7" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="O7" s="84" t="s">
+      <c r="O7" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="86"/>
+      <c r="P7" s="74"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="75"/>
-      <c r="C8" s="88"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -2687,28 +2686,28 @@
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M8" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N8" s="9">
         <v>1</v>
       </c>
-      <c r="O8" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="P8" s="79"/>
+      <c r="O8" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="76"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="75"/>
-      <c r="C9" s="88"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="104"/>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G9" s="14">
         <v>2</v>
@@ -2718,30 +2717,30 @@
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L9" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M9" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N9" s="21">
         <v>1</v>
       </c>
-      <c r="O9" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="P9" s="97"/>
+      <c r="O9" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="P9" s="95"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="66"/>
-      <c r="C10" s="89"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="105"/>
       <c r="D10" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G10" s="10">
         <v>3</v>
@@ -2751,34 +2750,34 @@
       </c>
       <c r="I10" s="12"/>
       <c r="J10" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M10" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N10" s="9">
         <v>1</v>
       </c>
-      <c r="O10" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="P10" s="79"/>
+      <c r="O10" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="P10" s="76"/>
     </row>
     <row r="11" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="65">
+      <c r="B11" s="78">
         <v>2</v>
       </c>
-      <c r="C11" s="87" t="s">
-        <v>99</v>
+      <c r="C11" s="103" t="s">
+        <v>115</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="G11" s="14">
         <v>4</v>
@@ -2788,30 +2787,30 @@
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L11" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="M11" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N11" s="21">
         <v>1</v>
       </c>
-      <c r="O11" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="P11" s="97"/>
+      <c r="O11" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="P11" s="95"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="75"/>
-      <c r="C12" s="88"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="10">
         <v>5</v>
@@ -2821,10 +2820,10 @@
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L12" s="40">
         <v>43830</v>
@@ -2835,16 +2834,16 @@
       <c r="N12" s="9">
         <v>1</v>
       </c>
-      <c r="O12" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="P12" s="79"/>
+      <c r="O12" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="P12" s="76"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="75"/>
-      <c r="C13" s="88"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="104"/>
       <c r="D13" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G13" s="14">
         <v>6</v>
@@ -2854,10 +2853,10 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K13" s="21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L13" s="41">
         <v>43831</v>
@@ -2868,16 +2867,16 @@
       <c r="N13" s="21">
         <v>1</v>
       </c>
-      <c r="O13" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="P13" s="97"/>
+      <c r="O13" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="P13" s="95"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="66"/>
-      <c r="C14" s="89"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="105"/>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G14" s="10">
         <v>7</v>
@@ -2887,10 +2886,10 @@
       </c>
       <c r="I14" s="12"/>
       <c r="J14" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L14" s="40">
         <v>55154</v>
@@ -2901,16 +2900,16 @@
       <c r="N14" s="9">
         <v>1</v>
       </c>
-      <c r="O14" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="P14" s="79"/>
+      <c r="O14" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14" s="76"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="65">
+      <c r="B15" s="78">
         <v>3</v>
       </c>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="103" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -2924,10 +2923,10 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K15" s="21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L15" s="41">
         <v>54789</v>
@@ -2938,14 +2937,14 @@
       <c r="N15" s="21">
         <v>1</v>
       </c>
-      <c r="O15" s="96" t="s">
-        <v>89</v>
-      </c>
-      <c r="P15" s="97"/>
+      <c r="O15" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="P15" s="95"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="75"/>
-      <c r="C16" s="88"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="104"/>
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
@@ -2959,12 +2958,12 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="96"/>
-      <c r="P16" s="97"/>
+      <c r="O16" s="94"/>
+      <c r="P16" s="95"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="75"/>
-      <c r="C17" s="88"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="104"/>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2978,12 +2977,12 @@
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="97"/>
+      <c r="O17" s="94"/>
+      <c r="P17" s="95"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="75"/>
-      <c r="C18" s="88"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="104"/>
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2997,12 +2996,12 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="96"/>
-      <c r="P18" s="97"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="95"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="75"/>
-      <c r="C19" s="88"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="104"/>
       <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
@@ -3016,21 +3015,21 @@
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
-      <c r="O19" s="96"/>
-      <c r="P19" s="97"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="95"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="66"/>
-      <c r="C20" s="89"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="105"/>
       <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="65">
+      <c r="B21" s="78">
         <v>4</v>
       </c>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="103" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -3038,64 +3037,70 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="75"/>
-      <c r="C22" s="88"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="104"/>
       <c r="D22" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="75"/>
-      <c r="C23" s="88"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="104"/>
       <c r="D23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24" s="75"/>
-      <c r="C24" s="88"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B25" s="75"/>
-      <c r="C25" s="88"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="66"/>
-      <c r="C26" s="89"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="105"/>
       <c r="D26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="92"/>
-      <c r="J26" s="92"/>
-      <c r="K26" s="92"/>
-      <c r="L26" s="92"/>
-      <c r="M26" s="92"/>
+      <c r="G26" s="99"/>
+      <c r="H26" s="99"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="100"/>
+      <c r="M26" s="100"/>
       <c r="N26" s="27"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="98"/>
       <c r="N27" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B11:B14"/>
     <mergeCell ref="I27:M27"/>
     <mergeCell ref="G5:P5"/>
     <mergeCell ref="B3:G3"/>
@@ -3112,18 +3117,12 @@
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="O17:P17"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3131,13 +3130,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="B1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
@@ -3155,69 +3154,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="69"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="125" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="104"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="126"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="K3" s="127"/>
       <c r="L3" s="44"/>
       <c r="M3" s="44"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="85" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="106" t="s">
+      <c r="C4" s="129" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="84" t="s">
+      <c r="F4" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="85"/>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="K4" s="85"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="111"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="105"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="136"/>
+      <c r="E5" s="128"/>
       <c r="F5" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="I5" s="16" t="s">
         <v>70</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>71</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>25</v>
@@ -3230,7 +3229,7 @@
       <c r="B6" s="15">
         <v>1</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="132" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="52" t="s">
@@ -3239,249 +3238,249 @@
       <c r="E6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="130" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="135" t="s">
-        <v>114</v>
-      </c>
-      <c r="H6" s="135" t="s">
-        <v>114</v>
+      <c r="F6" s="60" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="H6" s="65" t="s">
+        <v>110</v>
       </c>
       <c r="I6" s="45">
         <v>1</v>
       </c>
       <c r="J6" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K6" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B7" s="15">
         <v>2</v>
       </c>
-      <c r="C7" s="109"/>
+      <c r="C7" s="132"/>
       <c r="D7" s="53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="131" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" s="136" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="136" t="s">
-        <v>114</v>
+      <c r="F7" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" s="66" t="s">
+        <v>110</v>
       </c>
       <c r="I7" s="50">
         <v>1</v>
       </c>
       <c r="J7" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="K7" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B8" s="15">
         <v>3</v>
       </c>
-      <c r="C8" s="109"/>
+      <c r="C8" s="132"/>
       <c r="D8" s="42" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="130" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" s="135">
+      <c r="F8" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="65">
         <v>47463</v>
       </c>
-      <c r="H8" s="135">
+      <c r="H8" s="65">
         <v>47463</v>
       </c>
       <c r="I8" s="46">
         <v>1</v>
       </c>
       <c r="J8" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K8" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="15">
         <v>4</v>
       </c>
-      <c r="C9" s="109"/>
+      <c r="C9" s="132"/>
       <c r="D9" s="53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="131" t="s">
-        <v>116</v>
-      </c>
-      <c r="G9" s="136">
+      <c r="F9" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="G9" s="66">
         <v>45403</v>
       </c>
-      <c r="H9" s="136">
+      <c r="H9" s="66">
         <v>25568</v>
       </c>
       <c r="I9" s="50">
         <v>1</v>
       </c>
       <c r="J9" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K9" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="K9" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B10" s="15">
         <v>5</v>
       </c>
-      <c r="C10" s="109"/>
+      <c r="C10" s="132"/>
       <c r="D10" s="42" t="s">
         <v>28</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="131"/>
+        <v>80</v>
+      </c>
+      <c r="F10" s="61"/>
       <c r="G10" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I10" s="50">
         <v>1</v>
       </c>
       <c r="J10" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="K10" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="15">
         <v>6</v>
       </c>
-      <c r="C11" s="109"/>
+      <c r="C11" s="132"/>
       <c r="D11" s="42" t="s">
         <v>28</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="F11" s="132" t="s">
-        <v>117</v>
+        <v>91</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>113</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I11" s="46">
         <v>1</v>
       </c>
       <c r="J11" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K11" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B12" s="15">
         <v>7</v>
       </c>
-      <c r="C12" s="109"/>
+      <c r="C12" s="132"/>
       <c r="D12" s="42" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="133" t="s">
-        <v>75</v>
+      <c r="F12" s="63" t="s">
+        <v>74</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H12" s="40" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I12" s="50">
         <v>1</v>
       </c>
       <c r="J12" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="K12" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="15">
         <v>8</v>
       </c>
-      <c r="C13" s="109"/>
+      <c r="C13" s="132"/>
       <c r="D13" s="54" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="132" t="s">
-        <v>76</v>
+      <c r="F13" s="62" t="s">
+        <v>75</v>
       </c>
       <c r="G13" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="I13" s="48">
         <v>1</v>
       </c>
       <c r="J13" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K13" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15">
         <v>9</v>
       </c>
-      <c r="C14" s="109"/>
+      <c r="C14" s="132"/>
       <c r="D14" s="54" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="131" t="s">
-        <v>116</v>
+      <c r="F14" s="61" t="s">
+        <v>112</v>
       </c>
       <c r="G14" s="40">
         <v>43830</v>
@@ -3493,25 +3492,25 @@
         <v>1</v>
       </c>
       <c r="J14" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K14" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="K14" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B15" s="15">
         <v>10</v>
       </c>
-      <c r="C15" s="109"/>
+      <c r="C15" s="132"/>
       <c r="D15" s="54" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="134" t="s">
-        <v>116</v>
+        <v>82</v>
+      </c>
+      <c r="F15" s="64" t="s">
+        <v>112</v>
       </c>
       <c r="G15" s="41">
         <v>43831</v>
@@ -3523,25 +3522,25 @@
         <v>1</v>
       </c>
       <c r="J15" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K15" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B16" s="15">
         <v>11</v>
       </c>
-      <c r="C16" s="109"/>
+      <c r="C16" s="132"/>
       <c r="D16" s="54" t="s">
         <v>26</v>
       </c>
       <c r="E16" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="131" t="s">
-        <v>116</v>
+        <v>83</v>
+      </c>
+      <c r="F16" s="61" t="s">
+        <v>112</v>
       </c>
       <c r="G16" s="40">
         <v>55154</v>
@@ -3553,25 +3552,25 @@
         <v>1</v>
       </c>
       <c r="J16" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="K16" s="59" t="s">
         <v>93</v>
-      </c>
-      <c r="K16" s="59" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="15">
         <v>12</v>
       </c>
-      <c r="C17" s="110"/>
+      <c r="C17" s="133"/>
       <c r="D17" s="43" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="F17" s="134" t="s">
-        <v>116</v>
+        <v>84</v>
+      </c>
+      <c r="F17" s="64" t="s">
+        <v>112</v>
       </c>
       <c r="G17" s="41">
         <v>54789</v>
@@ -3583,10 +3582,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K17" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -3615,98 +3614,98 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
-      <c r="K19" s="108"/>
-      <c r="L19" s="108"/>
+      <c r="K19" s="131"/>
+      <c r="L19" s="131"/>
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M20" s="5"/>
     </row>
     <row r="21" spans="2:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="120" t="s">
+      <c r="C21" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="121"/>
-      <c r="E21" s="121"/>
-      <c r="F21" s="122"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="112"/>
       <c r="G21" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="H21" s="99" t="s">
+      <c r="H21" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="I21" s="100"/>
-      <c r="J21" s="100"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="99" t="s">
+      <c r="I21" s="114"/>
+      <c r="J21" s="114"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="115"/>
+      <c r="M21" s="113" t="s">
         <v>54</v>
       </c>
-      <c r="N21" s="100"/>
-      <c r="O21" s="100"/>
-      <c r="P21" s="101"/>
+      <c r="N21" s="114"/>
+      <c r="O21" s="114"/>
+      <c r="P21" s="115"/>
     </row>
     <row r="22" spans="2:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="116" t="s">
+      <c r="B22" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="117" t="s">
+      <c r="C22" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="118" t="s">
+      <c r="D22" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="118" t="s">
+      <c r="E22" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="119" t="s">
+      <c r="F22" s="107" t="s">
         <v>58</v>
       </c>
-      <c r="G22" s="127" t="s">
+      <c r="G22" s="120" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="123" t="s">
+      <c r="H22" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="I22" s="124"/>
-      <c r="J22" s="72" t="s">
+      <c r="I22" s="117"/>
+      <c r="J22" s="85" t="s">
         <v>55</v>
       </c>
-      <c r="K22" s="118" t="s">
+      <c r="K22" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="L22" s="119" t="s">
+      <c r="L22" s="107" t="s">
         <v>57</v>
       </c>
-      <c r="M22" s="128" t="s">
+      <c r="M22" s="108" t="s">
         <v>60</v>
       </c>
-      <c r="N22" s="118" t="s">
+      <c r="N22" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="O22" s="118" t="s">
+      <c r="O22" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="P22" s="119" t="s">
+      <c r="P22" s="107" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="116"/>
-      <c r="C23" s="117"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="127"/>
-      <c r="H23" s="125"/>
-      <c r="I23" s="126"/>
-      <c r="J23" s="74"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="119"/>
-      <c r="M23" s="129"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="119"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="124"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="87"/>
+      <c r="K23" s="106"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="109"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="107"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="26" t="s">
@@ -3727,10 +3726,10 @@
       <c r="G24" s="57">
         <v>1</v>
       </c>
-      <c r="H24" s="114" t="s">
-        <v>87</v>
-      </c>
-      <c r="I24" s="115"/>
+      <c r="H24" s="121" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" s="122"/>
       <c r="J24" s="2">
         <v>6</v>
       </c>
@@ -3741,7 +3740,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N24" s="2">
         <v>6</v>
@@ -3758,23 +3757,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="H21:L21"/>
-    <mergeCell ref="H22:I23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
     <mergeCell ref="M21:P21"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="F4:I4"/>
@@ -3786,6 +3768,23 @@
     <mergeCell ref="C6:C17"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="D4:D5"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="H21:L21"/>
+    <mergeCell ref="H22:I23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="J22:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3795,6 +3794,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F5F472198D7887469049920058585067" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5e76e8f6ca957e849a493f1baa4f4bb7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c46c0853-0d59-45c6-b517-3e25eac8cdf1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ddeb00cc2097713d6f56fe4f26be38f" ns2:_="">
     <xsd:import namespace="c46c0853-0d59-45c6-b517-3e25eac8cdf1"/>
@@ -3938,22 +3952,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{153A5999-B236-48B1-944C-C5EB94545735}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3969,21 +3985,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B0A340A-7B8D-463A-B976-63A023B5D9BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C125791C-CFF3-4EED-94B5-3CF568D8D264}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>